<commit_message>
Add DOB and POB to table
</commit_message>
<xml_diff>
--- a/beispiel_liste.xlsx
+++ b/beispiel_liste.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="94">
   <si>
     <t xml:space="preserve">VN</t>
   </si>
@@ -28,6 +28,12 @@
     <t xml:space="preserve">NN</t>
   </si>
   <si>
+    <t xml:space="preserve">DOB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POB</t>
+  </si>
+  <si>
     <t xml:space="preserve">AV</t>
   </si>
   <si>
@@ -79,6 +85,12 @@
     <t xml:space="preserve">Bowie</t>
   </si>
   <si>
+    <t xml:space="preserve">08.01.1947</t>
+  </si>
+  <si>
+    <t xml:space="preserve">London</t>
+  </si>
+  <si>
     <t xml:space="preserve">Religion</t>
   </si>
   <si>
@@ -91,6 +103,12 @@
     <t xml:space="preserve">Mercury</t>
   </si>
   <si>
+    <t xml:space="preserve">05.09.1946</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stone Town</t>
+  </si>
+  <si>
     <t xml:space="preserve">Beeindruckende Bühnenpräsenz.</t>
   </si>
   <si>
@@ -100,6 +118,12 @@
     <t xml:space="preserve">Joplin</t>
   </si>
   <si>
+    <t xml:space="preserve">19.01.1943</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Port Arthur</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ethik</t>
   </si>
   <si>
@@ -112,6 +136,12 @@
     <t xml:space="preserve">Cobain</t>
   </si>
   <si>
+    <t xml:space="preserve">20.02.1967</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aberdeen</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ruhig, aber sehr talentiert.</t>
   </si>
   <si>
@@ -121,6 +151,9 @@
     <t xml:space="preserve">Winhouse</t>
   </si>
   <si>
+    <t xml:space="preserve">14.09.1983</t>
+  </si>
+  <si>
     <t xml:space="preserve">Zeigt großes Interesse an Musik.</t>
   </si>
   <si>
@@ -130,6 +163,12 @@
     <t xml:space="preserve">Hendrix</t>
   </si>
   <si>
+    <t xml:space="preserve">27.11.1942</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seattle</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sehr einfallsreicher Schüler.</t>
   </si>
   <si>
@@ -139,6 +178,12 @@
     <t xml:space="preserve">Presley</t>
   </si>
   <si>
+    <t xml:space="preserve">08.01.1935</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tupelo</t>
+  </si>
+  <si>
     <t xml:space="preserve">Gute Mitarbeit und Motivation.</t>
   </si>
   <si>
@@ -148,6 +193,12 @@
     <t xml:space="preserve">Lennon</t>
   </si>
   <si>
+    <t xml:space="preserve">09.10.1940</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Liverpool</t>
+  </si>
+  <si>
     <t xml:space="preserve">Kreative Beiträge im Unterricht.</t>
   </si>
   <si>
@@ -157,6 +208,9 @@
     <t xml:space="preserve">Harrison</t>
   </si>
   <si>
+    <t xml:space="preserve">25.02.1943</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sehr freundlich zu Mitschülern.</t>
   </si>
   <si>
@@ -166,6 +220,12 @@
     <t xml:space="preserve">Morrison</t>
   </si>
   <si>
+    <t xml:space="preserve">08.12.1943</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Melbourne</t>
+  </si>
+  <si>
     <t xml:space="preserve">Manchmal unkonzentriert.</t>
   </si>
   <si>
@@ -175,6 +235,12 @@
     <t xml:space="preserve">Houston</t>
   </si>
   <si>
+    <t xml:space="preserve">09.08.1963</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Newark</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sehr engagiert, besonders in Musik.</t>
   </si>
   <si>
@@ -184,6 +250,12 @@
     <t xml:space="preserve">Shakur</t>
   </si>
   <si>
+    <t xml:space="preserve">16.06.1971</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New York</t>
+  </si>
+  <si>
     <t xml:space="preserve">Gute Mitarbeit, manchmal laut.</t>
   </si>
   <si>
@@ -193,6 +265,12 @@
     <t xml:space="preserve">Sinatra</t>
   </si>
   <si>
+    <t xml:space="preserve">12.12.1915</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hoboken</t>
+  </si>
+  <si>
     <t xml:space="preserve">Höflich und respektvoll.</t>
   </si>
   <si>
@@ -202,6 +280,12 @@
     <t xml:space="preserve">Rogers</t>
   </si>
   <si>
+    <t xml:space="preserve">07.06.1958</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minneapolis</t>
+  </si>
+  <si>
     <t xml:space="preserve">Zeigt außergewöhnliches Talent.</t>
   </si>
   <si>
@@ -209,6 +293,12 @@
   </si>
   <si>
     <t xml:space="preserve">Jackson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29.08.1958</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gary</t>
   </si>
   <si>
     <t xml:space="preserve">Tänzerisch und musikalisch begabt.</t>
@@ -307,30 +397,32 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q16"/>
+  <dimension ref="A1:S16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L17" activeCellId="0" sqref="L17"/>
+      <selection pane="topLeft" activeCell="O17" activeCellId="0" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="3.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="4.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="5.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="3.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="4.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="4.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="4.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="4.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="4.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="8.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="5.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="4.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="4.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="4.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="4.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="4.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="7.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="8.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="11.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="30.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="11.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="4.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="7.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="8.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="11.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="30.61"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -385,72 +477,84 @@
       <c r="Q1" s="0" t="s">
         <v>16</v>
       </c>
+      <c r="R1" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="0" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>1</v>
+        <v>20</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>22</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>2</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G2" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H2" s="0" t="n">
         <v>2</v>
       </c>
       <c r="I2" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J2" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K2" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="L2" s="0" t="s">
-        <v>19</v>
+        <v>3</v>
+      </c>
+      <c r="L2" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="M2" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="N2" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>23</v>
       </c>
       <c r="O2" s="0" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P2" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="Q2" s="0" t="s">
-        <v>20</v>
+      <c r="Q2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S2" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>1</v>
+        <v>26</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>28</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>1</v>
@@ -471,95 +575,107 @@
         <v>1</v>
       </c>
       <c r="K3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="L3" s="0" t="s">
-        <v>19</v>
+        <v>1</v>
+      </c>
+      <c r="L3" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="M3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="N3" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="N3" s="0" t="s">
+        <v>23</v>
       </c>
       <c r="O3" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q3" s="0" t="s">
-        <v>23</v>
+        <v>1</v>
+      </c>
+      <c r="Q3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="R3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="S3" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>2</v>
+        <v>31</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>33</v>
       </c>
       <c r="E4" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>2</v>
       </c>
       <c r="G4" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H4" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I4" s="0" t="n">
         <v>2</v>
       </c>
       <c r="J4" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="L4" s="0" t="s">
-        <v>26</v>
+        <v>2</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="M4" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="N4" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="N4" s="0" t="s">
+        <v>34</v>
       </c>
       <c r="O4" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P4" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="Q4" s="0" t="s">
-        <v>27</v>
+      <c r="Q4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S4" s="0" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>2</v>
+        <v>37</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>39</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>2</v>
@@ -574,42 +690,48 @@
         <v>2</v>
       </c>
       <c r="J5" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K5" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="L5" s="0" t="s">
-        <v>19</v>
+      <c r="L5" s="0" t="n">
+        <v>3</v>
       </c>
       <c r="M5" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="N5" s="0" t="n">
-        <v>2</v>
+        <v>2</v>
+      </c>
+      <c r="N5" s="0" t="s">
+        <v>23</v>
       </c>
       <c r="O5" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P5" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="0" t="s">
-        <v>30</v>
+        <v>2</v>
+      </c>
+      <c r="Q5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="S5" s="0" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D6" s="0" t="n">
-        <v>2</v>
+        <v>42</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>22</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>2</v>
@@ -618,51 +740,57 @@
         <v>2</v>
       </c>
       <c r="G6" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H6" s="0" t="n">
         <v>2</v>
       </c>
       <c r="I6" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J6" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K6" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="L6" s="0" t="s">
-        <v>19</v>
+        <v>2</v>
+      </c>
+      <c r="L6" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="M6" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="N6" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="N6" s="0" t="s">
+        <v>34</v>
       </c>
       <c r="O6" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P6" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q6" s="0" t="s">
-        <v>33</v>
+        <v>1</v>
+      </c>
+      <c r="Q6" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="R6" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="S6" s="0" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D7" s="0" t="n">
-        <v>1</v>
+        <v>46</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>48</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>1</v>
@@ -674,48 +802,54 @@
         <v>1</v>
       </c>
       <c r="H7" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I7" s="0" t="n">
         <v>1</v>
       </c>
       <c r="J7" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K7" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="L7" s="0" t="s">
-        <v>19</v>
+        <v>1</v>
+      </c>
+      <c r="L7" s="0" t="n">
+        <v>3</v>
       </c>
       <c r="M7" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="N7" s="0" t="n">
-        <v>0</v>
+      <c r="N7" s="0" t="s">
+        <v>23</v>
       </c>
       <c r="O7" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P7" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="Q7" s="0" t="s">
-        <v>36</v>
+      <c r="Q7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S7" s="0" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D8" s="0" t="n">
-        <v>1</v>
+        <v>51</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>53</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>1</v>
@@ -724,104 +858,116 @@
         <v>1</v>
       </c>
       <c r="G8" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H8" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I8" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J8" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K8" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="L8" s="0" t="s">
-        <v>26</v>
+        <v>1</v>
+      </c>
+      <c r="L8" s="0" t="n">
+        <v>2</v>
       </c>
       <c r="M8" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="N8" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="N8" s="0" t="s">
+        <v>23</v>
       </c>
       <c r="O8" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P8" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="Q8" s="0" t="s">
-        <v>39</v>
+      <c r="Q8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S8" s="0" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D9" s="0" t="n">
-        <v>1</v>
+        <v>56</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>58</v>
       </c>
       <c r="E9" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F9" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G9" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H9" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I9" s="0" t="n">
         <v>2</v>
       </c>
       <c r="J9" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K9" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="L9" s="0" t="s">
-        <v>19</v>
+        <v>2</v>
+      </c>
+      <c r="L9" s="0" t="n">
+        <v>2</v>
       </c>
       <c r="M9" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="N9" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="N9" s="0" t="s">
+        <v>23</v>
       </c>
       <c r="O9" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P9" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="Q9" s="0" t="s">
-        <v>42</v>
+      <c r="Q9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S9" s="0" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D10" s="0" t="n">
-        <v>2</v>
+        <v>61</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>58</v>
       </c>
       <c r="E10" s="0" t="n">
         <v>2</v>
@@ -839,48 +985,54 @@
         <v>2</v>
       </c>
       <c r="J10" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K10" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="L10" s="0" t="s">
-        <v>26</v>
+      <c r="L10" s="0" t="n">
+        <v>3</v>
       </c>
       <c r="M10" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="N10" s="0" t="n">
-        <v>1</v>
+      <c r="N10" s="0" t="s">
+        <v>34</v>
       </c>
       <c r="O10" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P10" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="Q10" s="0" t="s">
-        <v>45</v>
+      <c r="Q10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="S10" s="0" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="C11" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="D11" s="0" t="n">
-        <v>3</v>
+        <v>65</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>67</v>
       </c>
       <c r="E11" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F11" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G11" s="0" t="n">
         <v>2</v>
@@ -889,45 +1041,51 @@
         <v>2</v>
       </c>
       <c r="I11" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J11" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K11" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="L11" s="0" t="s">
-        <v>26</v>
+      <c r="L11" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="M11" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="N11" s="0" t="n">
-        <v>2</v>
+      <c r="N11" s="0" t="s">
+        <v>34</v>
       </c>
       <c r="O11" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P11" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="0" t="s">
-        <v>48</v>
+        <v>2</v>
+      </c>
+      <c r="Q11" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="R11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S11" s="0" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="C12" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D12" s="0" t="n">
-        <v>1</v>
+        <v>70</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>72</v>
       </c>
       <c r="E12" s="0" t="n">
         <v>1</v>
@@ -939,101 +1097,113 @@
         <v>1</v>
       </c>
       <c r="H12" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I12" s="0" t="n">
         <v>1</v>
       </c>
       <c r="J12" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K12" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="L12" s="0" t="s">
-        <v>26</v>
+      <c r="L12" s="0" t="n">
+        <v>3</v>
       </c>
       <c r="M12" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="N12" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="N12" s="0" t="s">
+        <v>23</v>
       </c>
       <c r="O12" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P12" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="Q12" s="0" t="s">
-        <v>51</v>
+      <c r="Q12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S12" s="0" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="C13" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D13" s="0" t="n">
-        <v>2</v>
+        <v>75</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>77</v>
       </c>
       <c r="E13" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F13" s="0" t="n">
         <v>2</v>
       </c>
       <c r="G13" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H13" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I13" s="0" t="n">
         <v>2</v>
       </c>
       <c r="J13" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K13" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="L13" s="0" t="s">
-        <v>19</v>
+        <v>2</v>
+      </c>
+      <c r="L13" s="0" t="n">
+        <v>2</v>
       </c>
       <c r="M13" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="N13" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="N13" s="0" t="s">
+        <v>34</v>
       </c>
       <c r="O13" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P13" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="0" t="s">
-        <v>54</v>
+        <v>1</v>
+      </c>
+      <c r="Q13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S13" s="0" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="C14" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D14" s="0" t="n">
-        <v>1</v>
+        <v>80</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>82</v>
       </c>
       <c r="E14" s="0" t="n">
         <v>1</v>
@@ -1042,10 +1212,10 @@
         <v>1</v>
       </c>
       <c r="G14" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H14" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I14" s="0" t="n">
         <v>2</v>
@@ -1054,92 +1224,104 @@
         <v>2</v>
       </c>
       <c r="K14" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="L14" s="0" t="s">
-        <v>19</v>
+        <v>2</v>
+      </c>
+      <c r="L14" s="0" t="n">
+        <v>2</v>
       </c>
       <c r="M14" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="N14" s="0" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="N14" s="0" t="s">
+        <v>34</v>
       </c>
       <c r="O14" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P14" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="Q14" s="0" t="s">
-        <v>57</v>
+      <c r="Q14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S14" s="0" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>58</v>
+        <v>84</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="C15" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D15" s="0" t="n">
-        <v>1</v>
+        <v>85</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>87</v>
       </c>
       <c r="E15" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F15" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G15" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H15" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I15" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J15" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K15" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="L15" s="0" t="s">
-        <v>26</v>
+        <v>1</v>
+      </c>
+      <c r="L15" s="0" t="n">
+        <v>3</v>
       </c>
       <c r="M15" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="N15" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="N15" s="0" t="s">
+        <v>23</v>
       </c>
       <c r="O15" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P15" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="Q15" s="0" t="s">
-        <v>60</v>
+      <c r="Q15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S15" s="0" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>61</v>
+        <v>89</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="C16" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D16" s="0" t="n">
-        <v>1</v>
+        <v>90</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>92</v>
       </c>
       <c r="E16" s="0" t="n">
         <v>1</v>
@@ -1151,34 +1333,40 @@
         <v>1</v>
       </c>
       <c r="H16" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I16" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J16" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K16" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="L16" s="0" t="s">
-        <v>26</v>
+      <c r="L16" s="0" t="n">
+        <v>3</v>
       </c>
       <c r="M16" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="N16" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="N16" s="0" t="s">
+        <v>23</v>
       </c>
       <c r="O16" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P16" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="Q16" s="0" t="s">
-        <v>63</v>
+      <c r="Q16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S16" s="0" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>